<commit_message>
Revisión de recursos aprovechados
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion03/Escaleta_LE_ 08_03_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion03/Escaleta_LE_ 08_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AULA PLANETA\PROCESO JUNIO 2015\GRADO OCTAVO\LE_08_03_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\Lenguaje\fuentes\contenidos\grado08\guion03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1360,18 +1360,36 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1425,24 +1443,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1751,8 +1751,8 @@
   <dimension ref="A1:U255"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,94 +1780,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="67" t="s">
         <v>282</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="71" t="s">
+      <c r="J1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="73" t="s">
+      <c r="M1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="73"/>
-      <c r="O1" s="61" t="s">
+      <c r="N1" s="79"/>
+      <c r="O1" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="61" t="s">
+      <c r="P1" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="81" t="s">
+      <c r="Q1" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="85" t="s">
+      <c r="R1" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="81" t="s">
+      <c r="S1" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="83" t="s">
+      <c r="T1" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="81" t="s">
+      <c r="U1" s="61" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="68"/>
+      <c r="A2" s="72"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="74"/>
       <c r="M2" s="7" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="82"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -2926,7 +2926,7 @@
         <v>214</v>
       </c>
       <c r="K20" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L20" s="45" t="s">
         <v>8</v>
@@ -3406,7 +3406,7 @@
         <v>226</v>
       </c>
       <c r="K28" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L28" s="45" t="s">
         <v>8</v>
@@ -4605,12 +4605,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4625,6 +4619,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>